<commit_message>
Added new CAPC design and included new system for generating helper lab excel sheets
Also includes various minor bugfixes and typo corrections
</commit_message>
<xml_diff>
--- a/core_plates/sw_src001_seedcore.xlsx
+++ b/core_plates/sw_src001_seedcore.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stellawang/Dropbox (HMS)/sequences/platelayouts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/Shih_Lab_Postdoc/research_projects/crisscross_code/core_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5AD48D-C7DD-2441-A3FB-9909697BEF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9E53AD-DBD6-0D4B-B9C7-DFA417085B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19780" yWindow="7420" windowWidth="31800" windowHeight="15000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Names" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="761">
   <si>
     <t>1</t>
   </si>
@@ -2314,6 +2314,9 @@
   </si>
   <si>
     <t>seedcore-socket-144c16-x15n4(h21-725_h16-53)</t>
+  </si>
+  <si>
+    <t>P3264 Seed cores part 2 (4 rows, each row is y.n0 - y.n16, total 4 x 17)</t>
   </si>
 </sst>
 </file>
@@ -2667,6 +2670,14 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2682,14 +2693,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3882,7 +3885,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="125" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4047,7 +4052,7 @@
       <c r="Y2" s="6" t="s">
         <v>571</v>
       </c>
-      <c r="Z2" s="19" t="s">
+      <c r="Z2" s="27" t="s">
         <v>25</v>
       </c>
     </row>
@@ -4127,7 +4132,7 @@
       <c r="Y3" s="6" t="s">
         <v>595</v>
       </c>
-      <c r="Z3" s="20"/>
+      <c r="Z3" s="28"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -4189,7 +4194,7 @@
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="20"/>
+      <c r="Z4" s="28"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -4253,8 +4258,8 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="12"/>
-      <c r="Z5" s="21" t="s">
-        <v>29</v>
+      <c r="Z5" s="29" t="s">
+        <v>760</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4319,7 +4324,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="12"/>
-      <c r="Z6" s="20"/>
+      <c r="Z6" s="28"/>
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -4383,7 +4388,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="12"/>
-      <c r="Z7" s="20"/>
+      <c r="Z7" s="28"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -4447,7 +4452,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="12"/>
-      <c r="Z8" s="20"/>
+      <c r="Z8" s="28"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -4527,7 +4532,7 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="12"/>
-      <c r="Z10" s="22" t="s">
+      <c r="Z10" s="30" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4579,7 +4584,7 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="12"/>
-      <c r="Z11" s="23"/>
+      <c r="Z11" s="31"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -4629,7 +4634,7 @@
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="12"/>
-      <c r="Z12" s="23"/>
+      <c r="Z12" s="31"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
@@ -4679,7 +4684,7 @@
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="12"/>
-      <c r="Z13" s="23"/>
+      <c r="Z13" s="31"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
@@ -4729,7 +4734,7 @@
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="12"/>
-      <c r="Z14" s="23"/>
+      <c r="Z14" s="31"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
@@ -4779,7 +4784,7 @@
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="12"/>
-      <c r="Z15" s="23"/>
+      <c r="Z15" s="31"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
@@ -4829,7 +4834,7 @@
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="12"/>
-      <c r="Z16" s="23"/>
+      <c r="Z16" s="31"/>
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
@@ -4879,7 +4884,7 @@
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="12"/>
-      <c r="Z17" s="23"/>
+      <c r="Z17" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4899,7 +4904,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5064,7 +5071,7 @@
       <c r="Y2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="Z2" s="19" t="s">
+      <c r="Z2" s="27" t="s">
         <v>25</v>
       </c>
     </row>
@@ -5144,7 +5151,7 @@
       <c r="Y3" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="Z3" s="20"/>
+      <c r="Z3" s="28"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -5206,7 +5213,7 @@
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="20"/>
+      <c r="Z4" s="28"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -5270,8 +5277,8 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="12"/>
-      <c r="Z5" s="21" t="s">
-        <v>29</v>
+      <c r="Z5" s="29" t="s">
+        <v>760</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5336,7 +5343,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="12"/>
-      <c r="Z6" s="20"/>
+      <c r="Z6" s="28"/>
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -5400,7 +5407,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="12"/>
-      <c r="Z7" s="20"/>
+      <c r="Z7" s="28"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -5464,7 +5471,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="12"/>
-      <c r="Z8" s="20"/>
+      <c r="Z8" s="28"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -5544,7 +5551,7 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="12"/>
-      <c r="Z10" s="22" t="s">
+      <c r="Z10" s="30" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5596,7 +5603,7 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="12"/>
-      <c r="Z11" s="23"/>
+      <c r="Z11" s="31"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -5646,7 +5653,7 @@
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="12"/>
-      <c r="Z12" s="23"/>
+      <c r="Z12" s="31"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
@@ -5696,7 +5703,7 @@
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="12"/>
-      <c r="Z13" s="23"/>
+      <c r="Z13" s="31"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
@@ -5746,7 +5753,7 @@
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="12"/>
-      <c r="Z14" s="23"/>
+      <c r="Z14" s="31"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
@@ -5796,7 +5803,7 @@
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="12"/>
-      <c r="Z15" s="23"/>
+      <c r="Z15" s="31"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
@@ -5846,7 +5853,7 @@
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="12"/>
-      <c r="Z16" s="23"/>
+      <c r="Z16" s="31"/>
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
@@ -5896,7 +5903,7 @@
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="12"/>
-      <c r="Z17" s="23"/>
+      <c r="Z17" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5916,7 +5923,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6081,7 +6090,7 @@
       <c r="Y2" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="Z2" s="19" t="s">
+      <c r="Z2" s="27" t="s">
         <v>25</v>
       </c>
     </row>
@@ -6161,7 +6170,7 @@
       <c r="Y3" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="Z3" s="20"/>
+      <c r="Z3" s="28"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -6223,7 +6232,7 @@
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="20"/>
+      <c r="Z4" s="28"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -6287,8 +6296,8 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="12"/>
-      <c r="Z5" s="21" t="s">
-        <v>29</v>
+      <c r="Z5" s="29" t="s">
+        <v>760</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -6353,7 +6362,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="12"/>
-      <c r="Z6" s="20"/>
+      <c r="Z6" s="28"/>
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -6417,7 +6426,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="12"/>
-      <c r="Z7" s="20"/>
+      <c r="Z7" s="28"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -6481,7 +6490,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="12"/>
-      <c r="Z8" s="20"/>
+      <c r="Z8" s="28"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -6561,7 +6570,7 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="12"/>
-      <c r="Z10" s="22" t="s">
+      <c r="Z10" s="30" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6613,7 +6622,7 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="12"/>
-      <c r="Z11" s="23"/>
+      <c r="Z11" s="31"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -6663,7 +6672,7 @@
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="12"/>
-      <c r="Z12" s="23"/>
+      <c r="Z12" s="31"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
@@ -6713,7 +6722,7 @@
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="12"/>
-      <c r="Z13" s="23"/>
+      <c r="Z13" s="31"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
@@ -6763,7 +6772,7 @@
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="12"/>
-      <c r="Z14" s="23"/>
+      <c r="Z14" s="31"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
@@ -6813,7 +6822,7 @@
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="12"/>
-      <c r="Z15" s="23"/>
+      <c r="Z15" s="31"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
@@ -6863,7 +6872,7 @@
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="12"/>
-      <c r="Z16" s="23"/>
+      <c r="Z16" s="31"/>
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
@@ -6913,7 +6922,7 @@
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="12"/>
-      <c r="Z17" s="23"/>
+      <c r="Z17" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7052,7 +7061,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="12"/>
-      <c r="Z2" s="19" t="s">
+      <c r="Z2" s="27" t="s">
         <v>25</v>
       </c>
     </row>
@@ -7084,7 +7093,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="12"/>
-      <c r="Z3" s="20"/>
+      <c r="Z3" s="28"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -7114,7 +7123,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="12"/>
-      <c r="Z4" s="20"/>
+      <c r="Z4" s="28"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
@@ -7144,7 +7153,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="12"/>
-      <c r="Z5" s="21" t="s">
+      <c r="Z5" s="29" t="s">
         <v>29</v>
       </c>
     </row>
@@ -7176,7 +7185,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="12"/>
-      <c r="Z6" s="20"/>
+      <c r="Z6" s="28"/>
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
@@ -7206,7 +7215,7 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="12"/>
-      <c r="Z7" s="20"/>
+      <c r="Z7" s="28"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
@@ -7236,7 +7245,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="12"/>
-      <c r="Z8" s="20"/>
+      <c r="Z8" s="28"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -7316,7 +7325,7 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="12"/>
-      <c r="Z10" s="22" t="s">
+      <c r="Z10" s="30" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7368,7 +7377,7 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="12"/>
-      <c r="Z11" s="23"/>
+      <c r="Z11" s="31"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -7418,7 +7427,7 @@
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="12"/>
-      <c r="Z12" s="23"/>
+      <c r="Z12" s="31"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
@@ -7468,7 +7477,7 @@
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="12"/>
-      <c r="Z13" s="23"/>
+      <c r="Z13" s="31"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
@@ -7518,7 +7527,7 @@
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="12"/>
-      <c r="Z14" s="23"/>
+      <c r="Z14" s="31"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
@@ -7568,7 +7577,7 @@
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
       <c r="Y15" s="12"/>
-      <c r="Z15" s="23"/>
+      <c r="Z15" s="31"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
@@ -7618,7 +7627,7 @@
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="12"/>
-      <c r="Z16" s="23"/>
+      <c r="Z16" s="31"/>
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
@@ -7668,7 +7677,7 @@
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
       <c r="Y17" s="12"/>
-      <c r="Z17" s="23"/>
+      <c r="Z17" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7688,7 +7697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6E31EB-B819-FE41-ABDA-9CF6DF0D3A66}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -7700,387 +7709,387 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="19" t="s">
         <v>467</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="20" t="s">
         <v>468</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="20" t="s">
         <v>469</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="20" t="s">
         <v>470</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="20" t="s">
         <v>471</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="20" t="s">
         <v>472</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="20" t="s">
         <v>473</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="20" t="s">
         <v>474</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="20" t="s">
         <v>475</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="20" t="s">
         <v>476</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="28"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="23"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="21" t="s">
         <v>477</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="22" t="s">
         <v>478</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="22" t="s">
         <v>479</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="22" t="s">
         <v>480</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="22" t="s">
         <v>481</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="22" t="s">
         <v>482</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="22" t="s">
         <v>483</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="22" t="s">
         <v>484</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="22" t="s">
         <v>485</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="22" t="s">
         <v>486</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="28"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="23"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="21" t="s">
         <v>487</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="22" t="s">
         <v>488</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="22" t="s">
         <v>489</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="22" t="s">
         <v>490</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="22" t="s">
         <v>491</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="22" t="s">
         <v>492</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="22" t="s">
         <v>493</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="22" t="s">
         <v>494</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="22" t="s">
         <v>495</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="22" t="s">
         <v>496</v>
       </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="28"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="23"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="21" t="s">
         <v>497</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="22" t="s">
         <v>498</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="22" t="s">
         <v>499</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="22" t="s">
         <v>500</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="22" t="s">
         <v>501</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="22" t="s">
         <v>502</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="22" t="s">
         <v>503</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="22" t="s">
         <v>504</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="22" t="s">
         <v>505</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="22" t="s">
         <v>506</v>
       </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="28"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="23"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="21" t="s">
         <v>507</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="22" t="s">
         <v>508</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="22" t="s">
         <v>509</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="22" t="s">
         <v>511</v>
       </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="22" t="s">
         <v>512</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="22" t="s">
         <v>513</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="22" t="s">
         <v>514</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="22" t="s">
         <v>515</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="22" t="s">
         <v>516</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="28"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="23"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="21" t="s">
         <v>517</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="22" t="s">
         <v>518</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="22" t="s">
         <v>519</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="22" t="s">
         <v>520</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="22" t="s">
         <v>521</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="22" t="s">
         <v>522</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="22" t="s">
         <v>523</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="22" t="s">
         <v>524</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="22" t="s">
         <v>525</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="22" t="s">
         <v>526</v>
       </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="28"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="23"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="21" t="s">
         <v>527</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="22" t="s">
         <v>528</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="22" t="s">
         <v>529</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="22" t="s">
         <v>530</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="22" t="s">
         <v>531</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="22" t="s">
         <v>532</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="22" t="s">
         <v>533</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="22" t="s">
         <v>534</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="22" t="s">
         <v>535</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="22" t="s">
         <v>536</v>
       </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="28"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="23"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="21" t="s">
         <v>537</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="22" t="s">
         <v>538</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="22" t="s">
         <v>539</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="22" t="s">
         <v>540</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="22" t="s">
         <v>541</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="22" t="s">
         <v>542</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="22" t="s">
         <v>543</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="22" t="s">
         <v>544</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="22" t="s">
         <v>545</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="22" t="s">
         <v>546</v>
       </c>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>